<commit_message>
adding grid to default
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/image_manifest.xlsx
+++ b/src/test/resources/bulk/image_manifest.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -90,7 +90,7 @@
     <t>admin</t>
   </si>
   <si>
-    <t>dateCreated</t>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Merge of grid into stable
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/image_manifest.xlsx
+++ b/src/test/resources/bulk/image_manifest.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -90,7 +90,7 @@
     <t>admin</t>
   </si>
   <si>
-    <t>dateCreated</t>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding harris to default
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/image_manifest.xlsx
+++ b/src/test/resources/bulk/image_manifest.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21930" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -21,9 +22,6 @@
     <t>5127663428_42ef7f4463_b.jpg</t>
   </si>
   <si>
-    <t>handbook_of_archaeology.jpg</t>
-  </si>
-  <si>
     <t>filename</t>
   </si>
   <si>
@@ -91,6 +89,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>HANDBOOK_of_archaeology.jpg</t>
   </si>
 </sst>
 </file>
@@ -108,17 +109,20 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -459,44 +463,47 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -507,62 +514,62 @@
         <v>1234</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>2222</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge of harris into stable
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/image_manifest.xlsx
+++ b/src/test/resources/bulk/image_manifest.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21930" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -21,9 +22,6 @@
     <t>5127663428_42ef7f4463_b.jpg</t>
   </si>
   <si>
-    <t>handbook_of_archaeology.jpg</t>
-  </si>
-  <si>
     <t>filename</t>
   </si>
   <si>
@@ -91,6 +89,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>HANDBOOK_of_archaeology.jpg</t>
   </si>
 </sst>
 </file>
@@ -108,17 +109,20 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -459,44 +463,47 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -507,62 +514,62 @@
         <v>1234</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>2222</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing bulk upload template  - extracting out template code into it's own bean  - adding validation for numeric and integer fields  - simplifying logic and basing more data on observation of the bean properties  - adding some comments
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/image_manifest.xlsx
+++ b/src/test/resources/bulk/image_manifest.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>5127663428_42ef7f4463_b.jpg</t>
   </si>
@@ -43,27 +42,9 @@
     <t>old book</t>
   </si>
   <si>
-    <t>ResourceCreator.Institution.name</t>
-  </si>
-  <si>
-    <t>ResourceCreator.role</t>
-  </si>
-  <si>
     <t>SPONSOR</t>
   </si>
   <si>
-    <t>ResourceCreator.Person.lastName</t>
-  </si>
-  <si>
-    <t>ResourceCreator.Person.firstName</t>
-  </si>
-  <si>
-    <t>ResourceCreator.Person.email</t>
-  </si>
-  <si>
-    <t>ResourceCreator.Person.Institution.name</t>
-  </si>
-  <si>
     <t>CREATOR</t>
   </si>
   <si>
@@ -92,6 +73,27 @@
   </si>
   <si>
     <t>HANDBOOK_of_archaeology.jpg</t>
+  </si>
+  <si>
+    <t>ResourceCreatorInstitution.Institution.name</t>
+  </si>
+  <si>
+    <t>ResourceCreatorInstitution.role</t>
+  </si>
+  <si>
+    <t>ResourceCreatorPerson.Person.lastName</t>
+  </si>
+  <si>
+    <t>ResourceCreatorPerson.Person.firstName</t>
+  </si>
+  <si>
+    <t>ResourceCreatorPerson.Person.email</t>
+  </si>
+  <si>
+    <t>ResourceCreatorPerson.Person.Institution.name</t>
+  </si>
+  <si>
+    <t>ResourceCreatorPerson.role</t>
   </si>
 </sst>
 </file>
@@ -463,7 +465,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +478,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -485,25 +487,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -522,24 +524,24 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>2222</v>
@@ -551,25 +553,25 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>